<commit_message>
Fixes for release to Kevin.
</commit_message>
<xml_diff>
--- a/pcb/vera-module bill of materials.xlsx
+++ b/pcb/vera-module bill of materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\vera-module\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{833E9758-D790-4E52-A48E-5714DF880097}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655BBD08-F226-44F6-AB5D-A990F8E384F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16476" yWindow="2988" windowWidth="10116" windowHeight="8964"/>
+    <workbookView xWindow="1248" yWindow="0" windowWidth="20856" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cmd16" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="113">
   <si>
     <t>Qty</t>
   </si>
@@ -46,9 +46,6 @@
     <t>R0603</t>
   </si>
   <si>
-    <t>R36</t>
-  </si>
-  <si>
     <t>R41</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>U6</t>
   </si>
   <si>
-    <t>R30, R31, R32, R33</t>
-  </si>
-  <si>
     <t>7A-8.000MAAE-T</t>
   </si>
   <si>
@@ -232,12 +226,6 @@
     <t>J4</t>
   </si>
   <si>
-    <t>FIDUCIAL</t>
-  </si>
-  <si>
-    <t>FD1, FD2, FD3</t>
-  </si>
-  <si>
     <t>HDR8X1</t>
   </si>
   <si>
@@ -356,12 +344,27 @@
   </si>
   <si>
     <t>9.31k</t>
+  </si>
+  <si>
+    <t>1.2k</t>
+  </si>
+  <si>
+    <t>R30, R31, R32</t>
+  </si>
+  <si>
+    <t>R33, R36</t>
+  </si>
+  <si>
+    <t>All resistors 1%.</t>
+  </si>
+  <si>
+    <t>Revision 1: R28, R29 (499 -&gt; 1.2k)  R33 (75 -&gt; 0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -498,7 +501,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -676,18 +679,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -851,17 +842,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1216,818 +1202,813 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A35" activeCellId="2" sqref="A30 A34 A35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="28" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="E17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
+        <v>4300</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2">
+        <v>75</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2">
+        <v>536</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>3</v>
+      </c>
+      <c r="B31" s="2">
+        <v>100</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>3</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>3</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1070</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>3</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2150</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>1</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>2</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>1</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>2</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>2</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="B43" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>1</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>3</v>
-      </c>
-      <c r="B19" s="3">
-        <v>4300</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>4</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>2</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>2</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>2</v>
-      </c>
-      <c r="B24" s="3">
-        <v>499</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>2</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>4</v>
-      </c>
-      <c r="B26" s="3">
-        <v>75</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>4</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>1</v>
-      </c>
-      <c r="B28" s="3">
-        <v>0</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
-        <v>3</v>
-      </c>
-      <c r="B30" s="3">
-        <v>536</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>1</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>3</v>
-      </c>
-      <c r="B32" s="3">
-        <v>100</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>3</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
-        <v>3</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1070</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
-        <v>3</v>
-      </c>
-      <c r="B35" s="3">
-        <v>2150</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
-        <v>1</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
-        <v>1</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
-        <v>1</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
-        <v>1</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
-        <v>1</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
-        <v>1</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
-        <v>1</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
-        <v>1</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
-        <v>2</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
-        <v>1</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
-        <v>1</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>60</v>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F46">
-    <sortCondition ref="E2:E46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F45">
+    <sortCondition ref="E2:E45"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>